<commit_message>
fix several bugs, still need to test
</commit_message>
<xml_diff>
--- a/Documents/test_upload.xlsx
+++ b/Documents/test_upload.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="1700" windowWidth="43340" windowHeight="27880" tabRatio="500"/>
+    <workbookView xWindow="4020" yWindow="440" windowWidth="43340" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test_upload" sheetId="2" r:id="rId1"/>
@@ -2936,7 +2936,7 @@
   <dimension ref="A1:U193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>